<commit_message>
Ver 6 - Special Letters and Trustee Sigs
</commit_message>
<xml_diff>
--- a/TestingHarness_EXPORT.XLSX
+++ b/TestingHarness_EXPORT.XLSX
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Development\Development Operations\wCohen\In-Progress Projects\Ack Letters\Ver 5 - Setting default sig by amount\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Development\Development Operations\wCohen\In-Progress Projects\Ack Letters\Ver 6 - Special Letters and Trustee Sigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="174">
   <si>
     <t>Gf_Check_date</t>
   </si>
@@ -532,10 +532,19 @@
     <t>Phase 5</t>
   </si>
   <si>
-    <t>Setting Line Spacing</t>
-  </si>
-  <si>
-    <t>DMQ1505</t>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>This is special because WE SAID SO</t>
+  </si>
+  <si>
+    <t>Board Member</t>
+  </si>
+  <si>
+    <t>DMQ1507</t>
+  </si>
+  <si>
+    <t>Appeal: DMQ1507, Emily Wroe Sig</t>
   </si>
 </sst>
 </file>
@@ -891,7 +900,7 @@
   <dimension ref="A1:AK21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,13 +1060,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C2" s="1">
         <v>42086</v>
       </c>
       <c r="D2" s="5">
-        <v>900</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1">
         <v>42086</v>
@@ -1072,10 +1081,10 @@
         <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="O2" t="s">
         <v>75</v>
@@ -2216,6 +2225,9 @@
       <c r="AA18" t="s">
         <v>106</v>
       </c>
+      <c r="AC18" t="s">
+        <v>171</v>
+      </c>
       <c r="AD18" t="s">
         <v>52</v>
       </c>
@@ -2375,8 +2387,11 @@
       <c r="F21" t="s">
         <v>35</v>
       </c>
+      <c r="G21" t="s">
+        <v>170</v>
+      </c>
       <c r="H21" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="J21" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Ver 7 - Mid Level Contact
</commit_message>
<xml_diff>
--- a/TestingHarness_EXPORT.XLSX
+++ b/TestingHarness_EXPORT.XLSX
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Development\Development Operations\wCohen\In-Progress Projects\Ack Letters\Ver 6 - Special Letters and Trustee Sigs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Development\Development Operations\wCohen\In-Progress Projects\Ack Letters\Ver 5 - Setting default sig by amount\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="171">
   <si>
     <t>Gf_Check_date</t>
   </si>
@@ -532,19 +532,10 @@
     <t>Phase 5</t>
   </si>
   <si>
-    <t>Special</t>
-  </si>
-  <si>
-    <t>This is special because WE SAID SO</t>
-  </si>
-  <si>
-    <t>Board Member</t>
-  </si>
-  <si>
-    <t>DMQ1507</t>
-  </si>
-  <si>
-    <t>Appeal: DMQ1507, Emily Wroe Sig</t>
+    <t>Setting Line Spacing</t>
+  </si>
+  <si>
+    <t>DMQ1505</t>
   </si>
 </sst>
 </file>
@@ -900,7 +891,7 @@
   <dimension ref="A1:AK21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,13 +1051,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C2" s="1">
         <v>42086</v>
       </c>
       <c r="D2" s="5">
-        <v>30</v>
+        <v>900</v>
       </c>
       <c r="E2" s="1">
         <v>42086</v>
@@ -1081,10 +1072,10 @@
         <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="N2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O2" t="s">
         <v>75</v>
@@ -2225,9 +2216,6 @@
       <c r="AA18" t="s">
         <v>106</v>
       </c>
-      <c r="AC18" t="s">
-        <v>171</v>
-      </c>
       <c r="AD18" t="s">
         <v>52</v>
       </c>
@@ -2387,11 +2375,8 @@
       <c r="F21" t="s">
         <v>35</v>
       </c>
-      <c r="G21" t="s">
-        <v>170</v>
-      </c>
       <c r="H21" t="s">
-        <v>169</v>
+        <v>47</v>
       </c>
       <c r="J21" t="s">
         <v>37</v>

</xml_diff>